<commit_message>
tai improve import export excel customer
</commit_message>
<xml_diff>
--- a/TMTDentalAPI/ClientApp/src/assets/files/Mau_File_KH.xlsx
+++ b/TMTDentalAPI/ClientApp/src/assets/files/Mau_File_KH.xlsx
@@ -80,25 +80,14 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Chọn 1 trong 3 :
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>- Nam
-- Nữ 
-- Khác</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hiển thị định dạng: Ngày/Tháng/Năm
+Nhưng nhập liệu nhập định dạng:
+Tháng/Ngày/Năm</t>
         </r>
       </text>
     </comment>
@@ -106,53 +95,78 @@
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Theo định dạng </t>
-        </r>
-        <r>
-          <rPr>
             <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>dd/mm/yyyy</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-hoặc
+          <t xml:space="preserve">Chọn 1 trong 3 :
 </t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>- Nam
+- Nữ 
+- Khác</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Ví dụ nếu chỉ có năm sinh thì nhập: </t>
+        </r>
+        <r>
+          <rPr>
             <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>dd.mm.yyyy</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-hoặc
+          <t xml:space="preserve">1992
+- </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Nếu có tháng và năm thì nhập: </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">8/1992
+- </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Nếu ngày sinh đầy đủ thì nhập:
 </t>
         </r>
         <r>
@@ -163,7 +177,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>dd-mm-yyyy</t>
+          <t>8/5/1992</t>
         </r>
       </text>
     </comment>
@@ -172,7 +186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Tên KH</t>
   </si>
@@ -216,7 +230,28 @@
     <t>Nữ</t>
   </si>
   <si>
-    <t>Kế toán</t>
+    <t>1992</t>
+  </si>
+  <si>
+    <t>Nguyễn Tuấn Anh</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>8/1990</t>
+  </si>
+  <si>
+    <t>0369835014</t>
+  </si>
+  <si>
+    <t>246/16 Độc Lập, Tân Thành, Tân Phú, HCM</t>
+  </si>
+  <si>
+    <t>Tiểu đường,Dị ứng thuốc</t>
+  </si>
+  <si>
+    <t>Ngày tạo</t>
   </si>
 </sst>
 </file>
@@ -224,7 +259,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -288,9 +323,9 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -598,77 +633,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6">
+        <v>43991</v>
+      </c>
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="6">
-        <v>33702</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="6">
+        <v>44012</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>